<commit_message>
Escaleta 5, con una corrección
Se modificó el nombre en los recursos de consolidación
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion05/ESCALETA_LE_06_05_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion05/ESCALETA_LE_06_05_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\CRISTIAN\PLANETA\NUEVO\ESCALETAS\Escaletas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\GitHub\Lenguaje\fuentes\contenidos\grado06\guion05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -778,9 +778,6 @@
     <t>Recurso M3B1-01</t>
   </si>
   <si>
-    <t>¿Qué es el género lírico?</t>
-  </si>
-  <si>
     <t>Actividad para reconocer los rasgos del género lírico y la poesía popular</t>
   </si>
   <si>
@@ -847,9 +844,6 @@
     <t>Actividad para reconocer modificadores en oraciones</t>
   </si>
   <si>
-    <t xml:space="preserve">La estructura de la oración </t>
-  </si>
-  <si>
     <t>Actividad para ejercitarse en el reconocimeinto de las partes de la oración</t>
   </si>
   <si>
@@ -865,9 +859,6 @@
     <t xml:space="preserve">Actividad para practicar el uso de los signos de interrogación al interior de las oraciones </t>
   </si>
   <si>
-    <t>Escribe los signos de interrogación y admiración</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Actividad para practicar la escritura de signos ortográficos en un texto</t>
   </si>
   <si>
@@ -883,9 +874,6 @@
     <t>Recurso elaborado por el autor anteriormente (LE_06_08_CO_REC140). Hay que revisarlo y adaptarlo.</t>
   </si>
   <si>
-    <t>¿Cómo usas los signos de interrogación y de admiración?</t>
-  </si>
-  <si>
     <t>Actividad para ejercitarse en el uso de signos de interrogación y de exclamación</t>
   </si>
   <si>
@@ -922,9 +910,6 @@
     <t>Recurso M12B-01</t>
   </si>
   <si>
-    <t>La intención comunicativa de las entrevistas</t>
-  </si>
-  <si>
     <t>Actividad para practicar la comprensión de entrevistas</t>
   </si>
   <si>
@@ -949,9 +934,6 @@
     <t>Recurso F13-01</t>
   </si>
   <si>
-    <t>La redacción de una entrevista</t>
-  </si>
-  <si>
     <t>Actividad de reflexión sobre los pasos necesarios para redactar entrevistas</t>
   </si>
   <si>
@@ -1016,6 +998,24 @@
   </si>
   <si>
     <t>DBA2, DBA11. Establecer algunas fases básicas para realziar una entrevista y solicitar con una ficha de actividad que el estudiante realice su propia entrevista</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: ¿Qué es el género lírico?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: La estructura de la oración </t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: ¿Cómo usas los signos de interrogación y de admiración?</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Escribe los signos de interrogación y admiración</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La intención comunicativa de las entrevistas</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La redacción de una entrevista</t>
   </si>
 </sst>
 </file>
@@ -1319,34 +1319,16 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1386,6 +1368,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1694,9 +1694,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,94 +1725,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="19" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="58"/>
+      <c r="O1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="T1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="61" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="19" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="59"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="53"/>
       <c r="M2" s="20" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -2088,7 +2088,7 @@
         <v>36</v>
       </c>
       <c r="O7" s="27" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="P7" s="27" t="s">
         <v>19</v>
@@ -2204,7 +2204,7 @@
       <c r="M9" s="25"/>
       <c r="N9" s="25"/>
       <c r="O9" s="27" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="P9" s="27" t="s">
         <v>19</v>
@@ -2263,7 +2263,7 @@
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="27" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="P10" s="27" t="s">
         <v>19</v>
@@ -2389,7 +2389,7 @@
         <v>35</v>
       </c>
       <c r="O12" s="27" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="P12" s="27" t="s">
         <v>19</v>
@@ -2439,7 +2439,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K13" s="23" t="s">
         <v>20</v>
@@ -2452,7 +2452,7 @@
         <v>31</v>
       </c>
       <c r="O13" s="27" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="P13" s="27" t="s">
         <v>19</v>
@@ -2493,7 +2493,7 @@
         <v>173</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H14" s="27">
         <v>12</v>
@@ -2502,7 +2502,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>20</v>
@@ -2515,7 +2515,7 @@
         <v>43</v>
       </c>
       <c r="O14" s="27" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="P14" s="27" t="s">
         <v>20</v>
@@ -2554,7 +2554,7 @@
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="31" t="s">
-        <v>243</v>
+        <v>317</v>
       </c>
       <c r="H15" s="27">
         <v>13</v>
@@ -2563,7 +2563,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K15" s="23" t="s">
         <v>20</v>
@@ -2576,7 +2576,7 @@
         <v>121</v>
       </c>
       <c r="O15" s="27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P15" s="27" t="s">
         <v>19</v>
@@ -2615,7 +2615,7 @@
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H16" s="27">
         <v>14</v>
@@ -2624,7 +2624,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K16" s="23" t="s">
         <v>20</v>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="N16" s="25"/>
       <c r="O16" s="27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P16" s="27" t="s">
         <v>19</v>
@@ -2652,7 +2652,7 @@
         <v>136</v>
       </c>
       <c r="T16" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U16" s="28" t="s">
         <v>137</v>
@@ -2678,7 +2678,7 @@
         <v>175</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H17" s="27">
         <v>15</v>
@@ -2687,7 +2687,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K17" s="23" t="s">
         <v>19</v>
@@ -2698,7 +2698,7 @@
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
       <c r="O17" s="27" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="P17" s="27" t="s">
         <v>19</v>
@@ -2739,7 +2739,7 @@
         <v>176</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H18" s="27">
         <v>16</v>
@@ -2748,7 +2748,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K18" s="23" t="s">
         <v>19</v>
@@ -2759,7 +2759,7 @@
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
       <c r="O18" s="27" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="P18" s="27" t="s">
         <v>19</v>
@@ -2800,7 +2800,7 @@
         <v>178</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H19" s="27">
         <v>17</v>
@@ -2809,7 +2809,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K19" s="23" t="s">
         <v>20</v>
@@ -2822,7 +2822,7 @@
         <v>50</v>
       </c>
       <c r="O19" s="27" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="P19" s="27" t="s">
         <v>19</v>
@@ -2837,7 +2837,7 @@
         <v>128</v>
       </c>
       <c r="T19" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U19" s="28" t="s">
         <v>130</v>
@@ -2872,7 +2872,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K20" s="23" t="s">
         <v>19</v>
@@ -2883,7 +2883,7 @@
       <c r="M20" s="25"/>
       <c r="N20" s="25"/>
       <c r="O20" s="27" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="P20" s="27" t="s">
         <v>19</v>
@@ -2924,7 +2924,7 @@
         <v>180</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H21" s="27">
         <v>19</v>
@@ -2933,7 +2933,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K21" s="23" t="s">
         <v>20</v>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="F22" s="22"/>
       <c r="G22" s="31" t="s">
-        <v>266</v>
+        <v>318</v>
       </c>
       <c r="H22" s="27">
         <v>20</v>
@@ -2994,7 +2994,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K22" s="23" t="s">
         <v>20</v>
@@ -3007,7 +3007,7 @@
         <v>121</v>
       </c>
       <c r="O22" s="27" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="P22" s="27" t="s">
         <v>19</v>
@@ -3044,7 +3044,7 @@
       <c r="E23" s="21"/>
       <c r="F23" s="22"/>
       <c r="G23" s="31" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H23" s="27">
         <v>21</v>
@@ -3053,7 +3053,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="33" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K23" s="23" t="s">
         <v>20</v>
@@ -3066,7 +3066,7 @@
       </c>
       <c r="N23" s="25"/>
       <c r="O23" s="27" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="P23" s="27" t="s">
         <v>19</v>
@@ -3114,7 +3114,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="33" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K24" s="23" t="s">
         <v>20</v>
@@ -3127,7 +3127,7 @@
         <v>25</v>
       </c>
       <c r="O24" s="27" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="P24" s="27" t="s">
         <v>19</v>
@@ -3188,7 +3188,7 @@
         <v>121</v>
       </c>
       <c r="O25" s="27" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="P25" s="27" t="s">
         <v>19</v>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="F26" s="22"/>
       <c r="G26" s="31" t="s">
-        <v>278</v>
+        <v>319</v>
       </c>
       <c r="H26" s="27">
         <v>24</v>
@@ -3236,7 +3236,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="33" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="K26" s="23" t="s">
         <v>20</v>
@@ -3249,7 +3249,7 @@
         <v>121</v>
       </c>
       <c r="O26" s="27" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="P26" s="27" t="s">
         <v>19</v>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="F27" s="22"/>
       <c r="G27" s="31" t="s">
-        <v>272</v>
+        <v>320</v>
       </c>
       <c r="H27" s="27">
         <v>25</v>
@@ -3297,7 +3297,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="33" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="K27" s="23" t="s">
         <v>19</v>
@@ -3308,7 +3308,7 @@
       <c r="M27" s="25"/>
       <c r="N27" s="25"/>
       <c r="O27" s="27" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="P27" s="27" t="s">
         <v>20</v>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="31" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="H28" s="27">
         <v>26</v>
@@ -3356,7 +3356,7 @@
         <v>19</v>
       </c>
       <c r="J28" s="33" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="K28" s="23" t="s">
         <v>20</v>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="N28" s="25"/>
       <c r="O28" s="27" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="P28" s="27" t="s">
         <v>19</v>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="31" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H29" s="27">
         <v>27</v>
@@ -3417,7 +3417,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="33" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="K29" s="23" t="s">
         <v>20</v>
@@ -3430,7 +3430,7 @@
         <v>46</v>
       </c>
       <c r="O29" s="27" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="P29" s="27" t="s">
         <v>20</v>
@@ -3445,7 +3445,7 @@
         <v>128</v>
       </c>
       <c r="T29" s="30" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="U29" s="28" t="s">
         <v>130</v>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="31" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H30" s="27">
         <v>28</v>
@@ -3478,7 +3478,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="33" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="K30" s="23" t="s">
         <v>20</v>
@@ -3491,7 +3491,7 @@
         <v>36</v>
       </c>
       <c r="O30" s="27" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="P30" s="27" t="s">
         <v>19</v>
@@ -3506,7 +3506,7 @@
         <v>128</v>
       </c>
       <c r="T30" s="30" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="U30" s="28" t="s">
         <v>130</v>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="31" t="s">
-        <v>291</v>
+        <v>321</v>
       </c>
       <c r="H31" s="27">
         <v>29</v>
@@ -3539,7 +3539,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="33" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>20</v>
@@ -3552,7 +3552,7 @@
         <v>121</v>
       </c>
       <c r="O31" s="27" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="P31" s="27" t="s">
         <v>19</v>
@@ -3591,7 +3591,7 @@
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="31" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H32" s="27">
         <v>30</v>
@@ -3600,7 +3600,7 @@
         <v>19</v>
       </c>
       <c r="J32" s="33" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="K32" s="23" t="s">
         <v>20</v>
@@ -3613,7 +3613,7 @@
       </c>
       <c r="N32" s="25"/>
       <c r="O32" s="27" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="P32" s="27" t="s">
         <v>19</v>
@@ -3628,7 +3628,7 @@
         <v>136</v>
       </c>
       <c r="T32" s="30" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="U32" s="28" t="s">
         <v>137</v>
@@ -3661,7 +3661,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="33" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="K33" s="23" t="s">
         <v>19</v>
@@ -3672,7 +3672,7 @@
       <c r="M33" s="25"/>
       <c r="N33" s="25"/>
       <c r="O33" s="27" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="P33" s="27" t="s">
         <v>19</v>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="31" t="s">
-        <v>300</v>
+        <v>322</v>
       </c>
       <c r="H34" s="27">
         <v>32</v>
@@ -3720,7 +3720,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="33" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="K34" s="23" t="s">
         <v>20</v>
@@ -3733,7 +3733,7 @@
         <v>121</v>
       </c>
       <c r="O34" s="27" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="P34" s="27" t="s">
         <v>19</v>
@@ -3770,7 +3770,7 @@
       <c r="E35" s="21"/>
       <c r="F35" s="22"/>
       <c r="G35" s="31" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H35" s="27">
         <v>33</v>
@@ -3779,7 +3779,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K35" s="23" t="s">
         <v>20</v>
@@ -3792,7 +3792,7 @@
         <v>119</v>
       </c>
       <c r="O35" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P35" s="27" t="s">
         <v>19</v>
@@ -3838,7 +3838,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="33" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K36" s="23" t="s">
         <v>19</v>
@@ -3849,7 +3849,7 @@
       <c r="M36" s="25"/>
       <c r="N36" s="25"/>
       <c r="O36" s="27" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="P36" s="27" t="s">
         <v>19</v>
@@ -3861,13 +3861,13 @@
         <v>138</v>
       </c>
       <c r="S36" s="28" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="T36" s="30" t="s">
         <v>218</v>
       </c>
       <c r="U36" s="28" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3886,7 +3886,7 @@
       <c r="E37" s="21"/>
       <c r="F37" s="22"/>
       <c r="G37" s="31" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H37" s="27">
         <v>35</v>
@@ -3895,7 +3895,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="33" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="K37" s="23" t="s">
         <v>20</v>
@@ -3908,7 +3908,7 @@
         <v>28</v>
       </c>
       <c r="O37" s="27" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="P37" s="27" t="s">
         <v>19</v>
@@ -3954,7 +3954,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="33" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="K38" s="23" t="s">
         <v>20</v>
@@ -3967,7 +3967,7 @@
       </c>
       <c r="N38" s="25"/>
       <c r="O38" s="27" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="P38" s="27" t="s">
         <v>19</v>
@@ -5224,6 +5224,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5238,12 +5244,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>